<commit_message>
Doc: Added cutomer Requirements for client feature.
</commit_message>
<xml_diff>
--- a/Requirments/CRS.xlsx
+++ b/Requirments/CRS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI material\QA\Online-Mobile-Store-WebSite\Requirments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE1037E-B755-4E6B-BFCC-F7A0CD978338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA34804-7206-45DE-9208-FB98E6037D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -157,13 +157,108 @@
   </si>
   <si>
     <t>CRS_Login_003</t>
+  </si>
+  <si>
+    <t>CRS_Client_001</t>
+  </si>
+  <si>
+    <t>CRS-SIQ_Client_001</t>
+  </si>
+  <si>
+    <t>CRS_Client_002</t>
+  </si>
+  <si>
+    <t>CRS_Client_003</t>
+  </si>
+  <si>
+    <t>CRS_Client_004</t>
+  </si>
+  <si>
+    <t>CRS_Client_005</t>
+  </si>
+  <si>
+    <t>The client should be able to add one or more products to a shopping cart for future purchase consideration.</t>
+  </si>
+  <si>
+    <t>The client should be able to finalize and place an order by confirming the cart contents and completing the checkout process.</t>
+  </si>
+  <si>
+    <t>Client should be able to do these functionalities :
+- view history of previous buys 
+- add products to cart 
+- review cart 
+- view checkout 
+- place order</t>
+  </si>
+  <si>
+    <t>CRS_Client_006</t>
+  </si>
+  <si>
+    <t>The client can view a complete history of their previous purchases including (product details, order dates,items purchased, price, 
+shipping address and order status).</t>
+  </si>
+  <si>
+    <t>CRS-SIQ_Client_002</t>
+  </si>
+  <si>
+    <t>The order date displayed in the purchase history shall follow the format: dd/mm/yy (e.g., 08/04/25)</t>
+  </si>
+  <si>
+    <t>CRS-SIQ_Client_003</t>
+  </si>
+  <si>
+    <t>The order date recorded and displayed should not be a future date. All dates must be equal to or earlier than the current date.</t>
+  </si>
+  <si>
+    <t>CRS-SIQ_Client_004</t>
+  </si>
+  <si>
+    <t>The client should be able to view and review the contents of their cart, including product names, quantities, prices, 
+and the ability to modify product count or remove items.</t>
+  </si>
+  <si>
+    <t>CRS_Client_007</t>
+  </si>
+  <si>
+    <t>CRS-SIQ_Client_005</t>
+  </si>
+  <si>
+    <t>The client shouldl be able to navigate to the checkout page to review the final list of items and choose the payment method (Cash Only)
+before confirming the purchase.</t>
+  </si>
+  <si>
+    <t>CRS-SIQ_Client_006</t>
+  </si>
+  <si>
+    <t>CRS_Client_008</t>
+  </si>
+  <si>
+    <t>After placing order confirmation message should appears "your orders placed successfully" and redirect to history of buys</t>
+  </si>
+  <si>
+    <t>CRS_Client_009</t>
+  </si>
+  <si>
+    <t>client id should consists of the last 6 numbers of national id</t>
+  </si>
+  <si>
+    <t>CRS-SIQ_Client_007</t>
+  </si>
+  <si>
+    <t>CRS-SIQ_Login_001</t>
+  </si>
+  <si>
+    <t>CRS-SIQ_Login_002</t>
+  </si>
+  <si>
+    <t>CRS-SIQ_Login_003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -219,6 +314,26 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -234,7 +349,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -285,16 +400,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -309,7 +436,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,214 +668,438 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" customWidth="1"/>
-    <col min="2" max="2" width="168.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.88671875" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="168.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="52.8" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:3" ht="54.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
+      <c r="C14" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
+      <c r="C15" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="C16" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="36.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="36.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="36.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="10"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="10"/>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="10"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="10"/>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="10"/>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="10"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="10"/>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="17"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="17"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="17"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="17"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="17"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="17"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="17"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="17"/>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="17"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="17"/>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="17"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="17"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="17"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="12"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Doc: updated coloumn ID from link ID to SIQ ID to be descrptive
</commit_message>
<xml_diff>
--- a/Requirments/CRS.xlsx
+++ b/Requirments/CRS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI9M-Testing\Core\QA\WorkShop\Online-Mobile-Store-WebSite\Requirments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD815ED-B6C9-45BE-995C-126EE9E904E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2799DFA0-DADE-401D-BB9B-372BEAD8BCD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Link ID</t>
-  </si>
-  <si>
     <t>CRS-SIQ_Reg_001</t>
   </si>
   <si>
@@ -306,6 +303,9 @@
   </si>
   <si>
     <t>If the supplier wants to add a new product the product data which is mandatory (product id, product price &amp; product version) and the optional data ( product photo, product platform)</t>
+  </si>
+  <si>
+    <t>SIQ ID</t>
   </si>
 </sst>
 </file>
@@ -743,465 +743,465 @@
   </sheetPr>
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" customWidth="1"/>
-    <col min="2" max="2" width="255.6640625" customWidth="1"/>
-    <col min="3" max="3" width="44.33203125" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="255.7109375" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="54.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="52.8" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
+      <c r="C14" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B15" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C15" s="10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
+    <row r="16" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B16" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C16" s="15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="13" t="s">
+    <row r="17" spans="1:3" ht="127.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="15" t="s">
+      <c r="B17" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="36.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="36.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="36.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="18" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="127.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="17" t="s">
+      <c r="C23" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="35.4" x14ac:dyDescent="0.35">
-      <c r="A18" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A19" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A21" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="19" t="s">
+      <c r="B24" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="35.4" x14ac:dyDescent="0.35">
-      <c r="A22" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="35.4" x14ac:dyDescent="0.35">
-      <c r="A23" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="18" t="s">
+      <c r="C24" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A24" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="21" t="s">
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B28" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C28" s="21" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="21" t="s">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B29" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C29" s="21" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="21" t="s">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B30" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C30" s="23" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="23" t="s">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B31" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="B31" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="C31" s="23" t="s">
+      <c r="C32" s="23" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="B32" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32" s="23" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
       <c r="B33" s="20"/>
       <c r="C33" s="16"/>
     </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16"/>
       <c r="B34" s="20"/>
       <c r="C34" s="16"/>
     </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="20"/>
       <c r="C35" s="16"/>
     </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
       <c r="B36" s="20"/>
       <c r="C36" s="16"/>
     </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
     </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
     </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
     </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
     </row>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
     </row>
-    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
     </row>
-    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
     </row>
-    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
     </row>
-    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
     </row>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
     </row>
-    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
     </row>
-    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
     </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
     </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
     </row>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12"/>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
     </row>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12"/>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>

</xml_diff>

<commit_message>
Doc: updated client requirements
</commit_message>
<xml_diff>
--- a/Requirments/CRS.xlsx
+++ b/Requirments/CRS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI9M-Testing\Core\QA\WorkShop\Online-Mobile-Store-WebSite\Requirments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC6B2A2-59FB-4261-AF37-28C34A8642B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9FCE6B-CFDB-4CC9-A895-2270EC3A87CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -213,10 +213,6 @@
     <t>CRS-SIQ_Client_004</t>
   </si>
   <si>
-    <t>The client should be able to view and review the contents of their cart, including product names, quantities, prices, 
-and the ability to modify product count or remove items.</t>
-  </si>
-  <si>
     <t>CRS_Client_007</t>
   </si>
   <si>
@@ -306,6 +302,10 @@
   </si>
   <si>
     <t>If the supplier wants to add a new product the product data which is mandatory (product id, product price &amp; product version) and the optional data ( product photo, product platform)</t>
+  </si>
+  <si>
+    <t>The client should be able to view and review the contents of their cart, including product names, quantities, prices, 
+and the ability to increment or decrement product count or remove items.</t>
   </si>
 </sst>
 </file>
@@ -743,18 +743,18 @@
   </sheetPr>
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" customWidth="1"/>
-    <col min="2" max="2" width="255.6640625" customWidth="1"/>
-    <col min="3" max="3" width="44.33203125" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="255.7109375" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -765,7 +765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -776,7 +776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -787,7 +787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
@@ -798,7 +798,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
@@ -809,7 +809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
@@ -820,7 +820,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="52.8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="54.75" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
@@ -831,7 +831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
@@ -842,7 +842,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>21</v>
       </c>
@@ -853,7 +853,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>22</v>
       </c>
@@ -864,7 +864,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>23</v>
       </c>
@@ -875,7 +875,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>24</v>
       </c>
@@ -886,7 +886,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>25</v>
       </c>
@@ -897,7 +897,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>42</v>
       </c>
@@ -905,10 +905,10 @@
         <v>39</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>43</v>
       </c>
@@ -916,10 +916,10 @@
         <v>40</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>44</v>
       </c>
@@ -927,10 +927,10 @@
         <v>41</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="127.8" customHeight="1" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="127.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>45</v>
       </c>
@@ -941,7 +941,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="35.4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="36.75" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>47</v>
       </c>
@@ -952,7 +952,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>48</v>
       </c>
@@ -963,7 +963,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>49</v>
       </c>
@@ -974,7 +974,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>50</v>
       </c>
@@ -985,29 +985,29 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="35.4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="36.75" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>54</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="35.4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="36.75" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>54</v>
       </c>
@@ -1015,193 +1015,193 @@
         <v>52</v>
       </c>
       <c r="C24" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="10" t="s">
+      <c r="B25" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="C25" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="10" t="s">
+      <c r="B26" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="C26" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B28" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C28" s="21" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="21" t="s">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B29" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C29" s="21" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="21" t="s">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B30" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C30" s="23" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="23" t="s">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B31" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="B31" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="C31" s="23" t="s">
+      <c r="C32" s="23" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="B32" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32" s="23" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
       <c r="B33" s="20"/>
       <c r="C33" s="16"/>
     </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16"/>
       <c r="B34" s="20"/>
       <c r="C34" s="16"/>
     </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="20"/>
       <c r="C35" s="16"/>
     </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
       <c r="B36" s="20"/>
       <c r="C36" s="16"/>
     </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
     </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
     </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
     </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
     </row>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
     </row>
-    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
     </row>
-    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
     </row>
-    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
     </row>
-    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
     </row>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
     </row>
-    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
     </row>
-    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
     </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
     </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
     </row>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12"/>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
     </row>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12"/>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>

</xml_diff>

<commit_message>
fix supplier reviews comments
</commit_message>
<xml_diff>
--- a/Requirments/CRS.xlsx
+++ b/Requirments/CRS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Requirments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI9M-Testing\Core\QA\WorkShop\Online-Mobile-Store-WebSite\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9FCE6B-CFDB-4CC9-A895-2270EC3A87CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91BB032-5D33-46F8-9CCD-0EEB4F382324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -286,26 +286,26 @@
     <t>CRS_supplier_006</t>
   </si>
   <si>
-    <t>Supplier can add product with data (product id,product photo, product price, product version, product platform)</t>
-  </si>
-  <si>
     <t>Supplier can update product by changing any of product data (product id,product photo, product price, product version, product platform) using product id</t>
   </si>
   <si>
     <t>Supplier can delete product with product id</t>
   </si>
   <si>
-    <t>Product Id follow ID convention [Brand/Category]_[ProductName]_[Color]_[Size/Version]</t>
-  </si>
-  <si>
     <t>There is an error message If the supplier enter product Id that is not correct "Invalid product Id"</t>
-  </si>
-  <si>
-    <t>If the supplier wants to add a new product the product data which is mandatory (product id, product price &amp; product version) and the optional data ( product photo, product platform)</t>
   </si>
   <si>
     <t>The client should be able to view and review the contents of their cart, including product names, quantities, prices, 
 and the ability to increment or decrement product count or remove items.</t>
+  </si>
+  <si>
+    <t>Product Id follow ID convention [Brand/Category]_[ProductName]_[Size/Version]</t>
+  </si>
+  <si>
+    <t>If the supplier wants to add a new product the product data which is mandatory (product id, product price, product version, product photo&amp; product platform)</t>
+  </si>
+  <si>
+    <t>Supplier can add product with data (product id,product photo, product price, product version, product platform [IOS &amp;Android] )</t>
   </si>
 </sst>
 </file>
@@ -743,18 +743,18 @@
   </sheetPr>
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1"/>
-    <col min="2" max="2" width="255.7109375" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" customWidth="1"/>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="255.6640625" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -765,7 +765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -776,7 +776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -787,7 +787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
@@ -798,7 +798,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
@@ -809,7 +809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
@@ -820,7 +820,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="54.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="52.8" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
@@ -831,7 +831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
@@ -842,7 +842,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>21</v>
       </c>
@@ -853,7 +853,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>22</v>
       </c>
@@ -864,7 +864,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>23</v>
       </c>
@@ -875,7 +875,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>24</v>
       </c>
@@ -886,7 +886,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>25</v>
       </c>
@@ -897,7 +897,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>42</v>
       </c>
@@ -908,7 +908,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>43</v>
       </c>
@@ -919,7 +919,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>44</v>
       </c>
@@ -930,7 +930,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="127.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="127.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
         <v>45</v>
       </c>
@@ -941,7 +941,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="36.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="35.4" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
         <v>47</v>
       </c>
@@ -952,7 +952,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
         <v>48</v>
       </c>
@@ -963,7 +963,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
         <v>49</v>
       </c>
@@ -974,7 +974,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
         <v>50</v>
       </c>
@@ -985,18 +985,18 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="36.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="35.4" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
         <v>54</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="36.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="35.4" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
         <v>61</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
         <v>54</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
         <v>64</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
         <v>66</v>
       </c>
@@ -1040,51 +1040,51 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="21" t="s">
         <v>79</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C27" s="21" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="21" t="s">
         <v>80</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C28" s="21" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="21" t="s">
         <v>81</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C29" s="21" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="23" t="s">
         <v>82</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C30" s="23" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="23" t="s">
         <v>83</v>
       </c>
@@ -1095,113 +1095,113 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="23" t="s">
         <v>84</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C32" s="23" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="20"/>
       <c r="C33" s="16"/>
     </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="20"/>
       <c r="C34" s="16"/>
     </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="16"/>
       <c r="B35" s="20"/>
       <c r="C35" s="16"/>
     </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="16"/>
       <c r="B36" s="20"/>
       <c r="C36" s="16"/>
     </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
     </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
     </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
     </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
     </row>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
     </row>
-    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
     </row>
-    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
     </row>
-    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="12"/>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
     </row>
-    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="12"/>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
     </row>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="12"/>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
     </row>
-    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="12"/>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
     </row>
-    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
     </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
     </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
     </row>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="12"/>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
     </row>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="12"/>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>

</xml_diff>

<commit_message>
Supplier fix review comments
</commit_message>
<xml_diff>
--- a/Requirments/CRS.xlsx
+++ b/Requirments/CRS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI material\QA\Online-Mobile-Store-WebSite\Requirments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI9M-Testing\Core\QA\WorkShop\Online-Mobile-Store-WebSite\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90780C79-E8AD-4A9E-9ADC-8DE32EFCA7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3B8794-A22D-4625-85DA-5F0A5D8CBEB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="92">
   <si>
     <t>ID</t>
   </si>
@@ -283,22 +283,13 @@
     <t>CRS_supplier_006</t>
   </si>
   <si>
-    <t>Supplier can add product with data (product id,product photo, product price, product version, product platform)</t>
-  </si>
-  <si>
     <t>Supplier can update product by changing any of product data (product id,product photo, product price, product version, product platform) using product id</t>
   </si>
   <si>
     <t>Supplier can delete product with product id</t>
   </si>
   <si>
-    <t>Product Id follow ID convention [Brand/Category]_[ProductName]_[Color]_[Size/Version]</t>
-  </si>
-  <si>
     <t>There is an error message If the supplier enter product Id that is not correct "Invalid product Id"</t>
-  </si>
-  <si>
-    <t>If the supplier wants to add a new product the product data which is mandatory (product id, product price &amp; product version) and the optional data ( product photo, product platform)</t>
   </si>
   <si>
     <t>The client should be able to view and review the contents of their cart, including product names, quantities, prices, 
@@ -306,6 +297,15 @@
   </si>
   <si>
     <t>when user enter invalid username or password or both error message shown is "please enter valid username or password"</t>
+  </si>
+  <si>
+    <t>Product Id follow ID convention [Brand/Category]_[ProductName]_[Size/Version]</t>
+  </si>
+  <si>
+    <t>Supplier can add product with data (product id,product photo, product price, product version, product platform [IOS&amp;Android] )</t>
+  </si>
+  <si>
+    <t>If the supplier wants to add a new product the product data which is mandatory (product id, product price , product version, product photo&amp; product platform)</t>
   </si>
 </sst>
 </file>
@@ -743,8 +743,8 @@
   </sheetPr>
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -924,7 +924,7 @@
         <v>43</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>70</v>
@@ -990,7 +990,7 @@
         <v>53</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>59</v>
@@ -1045,7 +1045,7 @@
         <v>78</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C27" s="21" t="s">
         <v>72</v>
@@ -1056,7 +1056,7 @@
         <v>79</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C28" s="21" t="s">
         <v>73</v>
@@ -1067,7 +1067,7 @@
         <v>80</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C29" s="21" t="s">
         <v>74</v>
@@ -1078,7 +1078,7 @@
         <v>81</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C30" s="23" t="s">
         <v>75</v>
@@ -1089,7 +1089,7 @@
         <v>82</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C31" s="23" t="s">
         <v>76</v>
@@ -1100,7 +1100,7 @@
         <v>83</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C32" s="23" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
Doc: updated requirments for the client Req
</commit_message>
<xml_diff>
--- a/Requirments/CRS.xlsx
+++ b/Requirments/CRS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0154186-0454-4BA2-82A6-2EABF661BDF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45B110C-9474-44DC-B494-E9050A3F41B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
   <si>
     <t>ID</t>
   </si>
@@ -313,6 +313,9 @@
   </si>
   <si>
     <t>If the cart is empty, a message "Your cart is empty." should be displayed.</t>
+  </si>
+  <si>
+    <t>CRS_Client_009</t>
   </si>
 </sst>
 </file>
@@ -750,8 +753,8 @@
   </sheetPr>
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1005,7 +1008,7 @@
     </row>
     <row r="23" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>88</v>
@@ -1016,7 +1019,7 @@
     </row>
     <row r="24" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B24" s="20" t="s">
         <v>60</v>
@@ -1027,7 +1030,7 @@
     </row>
     <row r="25" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
update CRS, SRS, RTM, Test Cases for client module
</commit_message>
<xml_diff>
--- a/Requirments/CRS.xlsx
+++ b/Requirments/CRS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Requirments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI9M-Testing\Core\QA\WorkShop\Online-Mobile-Store-WebSite\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4666970E-812D-4B85-BDCE-945E2DFA61E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E18E269-B98D-4D8B-881D-A494FB0F6DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -753,18 +753,18 @@
   </sheetPr>
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1"/>
-    <col min="2" max="2" width="255.7109375" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" customWidth="1"/>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="255.6640625" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -775,7 +775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -786,7 +786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -797,7 +797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
@@ -808,7 +808,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
@@ -819,7 +819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
@@ -830,7 +830,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="54.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="52.8" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
@@ -841,7 +841,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
@@ -852,7 +852,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>21</v>
       </c>
@@ -863,7 +863,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>22</v>
       </c>
@@ -874,7 +874,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>23</v>
       </c>
@@ -885,7 +885,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>24</v>
       </c>
@@ -896,7 +896,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>25</v>
       </c>
@@ -907,7 +907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>41</v>
       </c>
@@ -918,7 +918,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>42</v>
       </c>
@@ -929,7 +929,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>43</v>
       </c>
@@ -940,7 +940,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="127.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="127.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
         <v>44</v>
       </c>
@@ -951,7 +951,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>46</v>
       </c>
@@ -962,7 +962,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
         <v>47</v>
       </c>
@@ -973,7 +973,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
         <v>48</v>
       </c>
@@ -984,7 +984,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>49</v>
       </c>
@@ -995,7 +995,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>51</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
         <v>56</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>59</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
         <v>90</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="21" t="s">
         <v>73</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="21" t="s">
         <v>74</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="21" t="s">
         <v>75</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="23" t="s">
         <v>76</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" s="23" t="s">
         <v>77</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="23" t="s">
         <v>78</v>
       </c>
@@ -1105,102 +1105,102 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="16"/>
       <c r="B32" s="20"/>
       <c r="C32" s="16"/>
     </row>
-    <row r="33" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="20"/>
       <c r="C33" s="16"/>
     </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="20"/>
       <c r="C34" s="16"/>
     </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="16"/>
       <c r="B35" s="20"/>
       <c r="C35" s="16"/>
     </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
     </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
     </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
     </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
     </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
     </row>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
     </row>
-    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
     </row>
-    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
     </row>
-    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="12"/>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
     </row>
-    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="12"/>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
     </row>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="12"/>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
     </row>
-    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="12"/>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
     </row>
-    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
     </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
     </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
     </row>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="12"/>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>

</xml_diff>